<commit_message>
Update data with December/2020 production.
</commit_message>
<xml_diff>
--- a/anfavea_data_analysis.xlsx
+++ b/anfavea_data_analysis.xlsx
@@ -581,7 +581,7 @@
         <v>686</v>
       </c>
       <c r="Q2" t="n">
-        <v>0</v>
+        <v>708</v>
       </c>
     </row>
     <row r="3">
@@ -644,7 +644,7 @@
         <v>1202</v>
       </c>
       <c r="Q3" t="n">
-        <v>0</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="4">
@@ -707,7 +707,7 @@
         <v>152</v>
       </c>
       <c r="Q4" t="n">
-        <v>0</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5">
@@ -770,7 +770,7 @@
         <v>2254</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>3178</v>
       </c>
     </row>
     <row r="6">
@@ -833,7 +833,7 @@
         <v>355</v>
       </c>
       <c r="Q6" t="n">
-        <v>0</v>
+        <v>583</v>
       </c>
     </row>
     <row r="7">
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="Q8" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
@@ -1022,7 +1022,7 @@
         <v>6</v>
       </c>
       <c r="Q9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -1085,7 +1085,7 @@
         <v>20464</v>
       </c>
       <c r="Q10" t="n">
-        <v>0</v>
+        <v>20312</v>
       </c>
     </row>
     <row r="11">
@@ -1148,7 +1148,7 @@
         <v>12708</v>
       </c>
       <c r="Q11" t="n">
-        <v>0</v>
+        <v>14849</v>
       </c>
     </row>
     <row r="12">
@@ -1211,7 +1211,7 @@
         <v>12587</v>
       </c>
       <c r="Q12" t="n">
-        <v>0</v>
+        <v>14027</v>
       </c>
     </row>
     <row r="13">
@@ -1274,7 +1274,7 @@
         <v>35129</v>
       </c>
       <c r="Q13" t="n">
-        <v>0</v>
+        <v>38645</v>
       </c>
     </row>
     <row r="14">
@@ -1337,7 +1337,7 @@
         <v>8931</v>
       </c>
       <c r="Q14" t="n">
-        <v>0</v>
+        <v>9646</v>
       </c>
     </row>
     <row r="15">
@@ -1400,7 +1400,7 @@
         <v>872</v>
       </c>
       <c r="Q15" t="n">
-        <v>0</v>
+        <v>820</v>
       </c>
     </row>
     <row r="16">
@@ -1463,7 +1463,7 @@
         <v>227</v>
       </c>
       <c r="Q16" t="n">
-        <v>0</v>
+        <v>221</v>
       </c>
     </row>
     <row r="17">
@@ -1526,7 +1526,7 @@
         <v>17388</v>
       </c>
       <c r="Q17" t="n">
-        <v>0</v>
+        <v>20257</v>
       </c>
     </row>
     <row r="18">
@@ -1589,7 +1589,7 @@
         <v>44</v>
       </c>
       <c r="Q18" t="n">
-        <v>0</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19">
@@ -1652,7 +1652,7 @@
         <v>243</v>
       </c>
       <c r="Q19" t="n">
-        <v>0</v>
+        <v>273</v>
       </c>
     </row>
     <row r="20">
@@ -1715,7 +1715,7 @@
         <v>563</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>698</v>
       </c>
     </row>
     <row r="21">
@@ -1778,7 +1778,7 @@
         <v>4782</v>
       </c>
       <c r="Q21" t="n">
-        <v>0</v>
+        <v>5179</v>
       </c>
     </row>
     <row r="22">
@@ -1841,7 +1841,7 @@
         <v>1449</v>
       </c>
       <c r="Q22" t="n">
-        <v>0</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="23">
@@ -1904,7 +1904,7 @@
         <v>1036</v>
       </c>
       <c r="Q23" t="n">
-        <v>0</v>
+        <v>688</v>
       </c>
     </row>
     <row r="24">
@@ -1967,7 +1967,7 @@
         <v>11639</v>
       </c>
       <c r="Q24" t="n">
-        <v>0</v>
+        <v>13828</v>
       </c>
     </row>
     <row r="25">
@@ -2030,7 +2030,7 @@
         <v>11762</v>
       </c>
       <c r="Q25" t="n">
-        <v>0</v>
+        <v>12331</v>
       </c>
     </row>
     <row r="26">
@@ -2093,7 +2093,7 @@
         <v>42</v>
       </c>
       <c r="Q26" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27">
@@ -2156,7 +2156,7 @@
         <v>31022</v>
       </c>
       <c r="Q27" t="n">
-        <v>0</v>
+        <v>33458</v>
       </c>
     </row>
     <row r="28">
@@ -2219,7 +2219,7 @@
         <v>1983</v>
       </c>
       <c r="Q28" t="n">
-        <v>0</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="29">
@@ -2282,7 +2282,7 @@
         <v>293</v>
       </c>
       <c r="Q29" t="n">
-        <v>0</v>
+        <v>395</v>
       </c>
     </row>
     <row r="30">
@@ -2408,7 +2408,7 @@
         <v>18981</v>
       </c>
       <c r="Q31" t="n">
-        <v>0</v>
+        <v>19426</v>
       </c>
     </row>
     <row r="32">
@@ -2471,7 +2471,7 @@
         <v>2323</v>
       </c>
       <c r="Q32" t="n">
-        <v>0</v>
+        <v>2404</v>
       </c>
     </row>
     <row r="33">
@@ -2534,7 +2534,7 @@
         <v>4093</v>
       </c>
       <c r="Q33" t="n">
-        <v>0</v>
+        <v>3569</v>
       </c>
     </row>
     <row r="34">
@@ -2597,7 +2597,7 @@
         <v>901</v>
       </c>
       <c r="Q34" t="n">
-        <v>0</v>
+        <v>695</v>
       </c>
     </row>
     <row r="35">
@@ -2660,7 +2660,7 @@
         <v>286</v>
       </c>
       <c r="Q35" t="n">
-        <v>0</v>
+        <v>288</v>
       </c>
     </row>
     <row r="36">
@@ -2786,7 +2786,7 @@
         <v>334</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38">
@@ -2849,7 +2849,7 @@
         <v>606</v>
       </c>
       <c r="Q38" t="n">
-        <v>0</v>
+        <v>658</v>
       </c>
     </row>
     <row r="39">
@@ -2912,7 +2912,7 @@
         <v>735</v>
       </c>
       <c r="Q39" t="n">
-        <v>0</v>
+        <v>957</v>
       </c>
     </row>
     <row r="40">
@@ -2975,7 +2975,7 @@
         <v>406</v>
       </c>
       <c r="Q40" t="n">
-        <v>0</v>
+        <v>281</v>
       </c>
     </row>
     <row r="41">
@@ -3038,7 +3038,7 @@
         <v>148</v>
       </c>
       <c r="Q41" t="n">
-        <v>0</v>
+        <v>184</v>
       </c>
     </row>
     <row r="42">
@@ -3101,7 +3101,7 @@
         <v>1174</v>
       </c>
       <c r="Q42" t="n">
-        <v>0</v>
+        <v>1405</v>
       </c>
     </row>
     <row r="43">
@@ -3164,7 +3164,7 @@
         <v>3050</v>
       </c>
       <c r="Q43" t="n">
-        <v>0</v>
+        <v>3306</v>
       </c>
     </row>
     <row r="44">
@@ -3227,7 +3227,7 @@
         <v>3322</v>
       </c>
       <c r="Q44" t="n">
-        <v>0</v>
+        <v>4218</v>
       </c>
     </row>
     <row r="45">
@@ -3290,7 +3290,7 @@
         <v>257</v>
       </c>
       <c r="Q45" t="n">
-        <v>0</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46">
@@ -3353,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="Q46" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47">
@@ -3416,7 +3416,7 @@
         <v>194</v>
       </c>
       <c r="Q47" t="n">
-        <v>0</v>
+        <v>283</v>
       </c>
     </row>
     <row r="48">
@@ -3542,7 +3542,7 @@
         <v>66</v>
       </c>
       <c r="Q49" t="n">
-        <v>0</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50">
@@ -3605,7 +3605,7 @@
         <v>50</v>
       </c>
       <c r="Q50" t="n">
-        <v>0</v>
+        <v>54</v>
       </c>
     </row>
     <row r="51">
@@ -3668,7 +3668,7 @@
         <v>208</v>
       </c>
       <c r="Q51" t="n">
-        <v>0</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52">
@@ -3731,7 +3731,7 @@
         <v>3</v>
       </c>
       <c r="Q52" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53">
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="Q54" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
@@ -3920,7 +3920,7 @@
         <v>2</v>
       </c>
       <c r="Q55" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56">
@@ -3983,7 +3983,7 @@
         <v>25</v>
       </c>
       <c r="Q56" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="57">
@@ -4046,7 +4046,7 @@
         <v>3</v>
       </c>
       <c r="Q57" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -4109,7 +4109,7 @@
         <v>85</v>
       </c>
       <c r="Q58" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="59">
@@ -4172,7 +4172,7 @@
         <v>340</v>
       </c>
       <c r="Q59" t="n">
-        <v>0</v>
+        <v>319</v>
       </c>
     </row>
     <row r="60">
@@ -4235,7 +4235,7 @@
         <v>408</v>
       </c>
       <c r="Q60" t="n">
-        <v>0</v>
+        <v>533</v>
       </c>
     </row>
     <row r="61">
@@ -4298,7 +4298,7 @@
         <v>0</v>
       </c>
       <c r="Q61" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62">
@@ -4361,7 +4361,7 @@
         <v>1</v>
       </c>
       <c r="Q62" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
@@ -4487,7 +4487,7 @@
         <v>1</v>
       </c>
       <c r="Q64" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="65">
@@ -4550,7 +4550,7 @@
         <v>48</v>
       </c>
       <c r="Q65" t="n">
-        <v>0</v>
+        <v>56</v>
       </c>
     </row>
     <row r="66">
@@ -4613,7 +4613,7 @@
         <v>565</v>
       </c>
       <c r="Q66" t="n">
-        <v>0</v>
+        <v>484</v>
       </c>
     </row>
     <row r="67">
@@ -4676,7 +4676,7 @@
         <v>254</v>
       </c>
       <c r="Q67" t="n">
-        <v>0</v>
+        <v>183</v>
       </c>
     </row>
     <row r="68">
@@ -4928,7 +4928,7 @@
         <v>3</v>
       </c>
       <c r="Q71" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72">
@@ -4991,7 +4991,7 @@
         <v>183</v>
       </c>
       <c r="Q72" t="n">
-        <v>0</v>
+        <v>234</v>
       </c>
     </row>
     <row r="73">
@@ -5054,7 +5054,7 @@
         <v>1264</v>
       </c>
       <c r="Q73" t="n">
-        <v>0</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="74">
@@ -5117,7 +5117,7 @@
         <v>808</v>
       </c>
       <c r="Q74" t="n">
-        <v>0</v>
+        <v>891</v>
       </c>
     </row>
     <row r="75">
@@ -5180,7 +5180,7 @@
         <v>2</v>
       </c>
       <c r="Q75" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76">
@@ -5243,7 +5243,7 @@
         <v>194</v>
       </c>
       <c r="Q76" t="n">
-        <v>0</v>
+        <v>230</v>
       </c>
     </row>
     <row r="77">
@@ -5306,7 +5306,7 @@
         <v>0</v>
       </c>
       <c r="Q77" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
@@ -5369,7 +5369,7 @@
         <v>351</v>
       </c>
       <c r="Q78" t="n">
-        <v>0</v>
+        <v>286</v>
       </c>
     </row>
     <row r="79">
@@ -5495,7 +5495,7 @@
         <v>115</v>
       </c>
       <c r="Q80" t="n">
-        <v>0</v>
+        <v>131</v>
       </c>
     </row>
     <row r="81">
@@ -5558,7 +5558,7 @@
         <v>279</v>
       </c>
       <c r="Q81" t="n">
-        <v>0</v>
+        <v>243</v>
       </c>
     </row>
     <row r="82">
@@ -5684,7 +5684,7 @@
         <v>1425</v>
       </c>
       <c r="Q83" t="n">
-        <v>0</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="84">
@@ -5747,7 +5747,7 @@
         <v>1010</v>
       </c>
       <c r="Q84" t="n">
-        <v>0</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="85">
@@ -5810,7 +5810,7 @@
         <v>1248</v>
       </c>
       <c r="Q85" t="n">
-        <v>0</v>
+        <v>1525</v>
       </c>
     </row>
     <row r="86">
@@ -5873,7 +5873,7 @@
         <v>0</v>
       </c>
       <c r="Q86" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
@@ -5936,7 +5936,7 @@
         <v>132</v>
       </c>
       <c r="Q87" t="n">
-        <v>0</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88">
@@ -5999,7 +5999,7 @@
         <v>140</v>
       </c>
       <c r="Q88" t="n">
-        <v>0</v>
+        <v>137</v>
       </c>
     </row>
     <row r="89">
@@ -6062,7 +6062,7 @@
         <v>547</v>
       </c>
       <c r="Q89" t="n">
-        <v>0</v>
+        <v>372</v>
       </c>
     </row>
     <row r="90">
@@ -6125,7 +6125,7 @@
         <v>491</v>
       </c>
       <c r="Q90" t="n">
-        <v>0</v>
+        <v>359</v>
       </c>
     </row>
     <row r="91">
@@ -6188,7 +6188,7 @@
         <v>42</v>
       </c>
       <c r="Q91" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
     </row>
     <row r="92">
@@ -6251,7 +6251,7 @@
         <v>12</v>
       </c>
       <c r="Q92" t="n">
-        <v>0</v>
+        <v>52</v>
       </c>
     </row>
     <row r="93">
@@ -6314,7 +6314,7 @@
         <v>17</v>
       </c>
       <c r="Q93" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>